<commit_message>
Update outputs after ba94af9
</commit_message>
<xml_diff>
--- a/processed-data/rdata/spe/12_spatial_registration_sn/sn_spatial_annotations.xlsx
+++ b/processed-data/rdata/spe/12_spatial_registration_sn/sn_spatial_annotations.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Key" r:id="rId3" sheetId="1"/>
     <sheet name="annotation" r:id="rId4" sheetId="2"/>
     <sheet name="cor_layer" r:id="rId5" sheetId="3"/>
-    <sheet name="cor_k9" r:id="rId6" sheetId="4"/>
+    <sheet name="cor_k09" r:id="rId6" sheetId="4"/>
     <sheet name="cor_k16" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
@@ -30,7 +30,7 @@
     <t>cor_layer</t>
   </si>
   <si>
-    <t>cor_k9</t>
+    <t>cor_k09</t>
   </si>
   <si>
     <t>cor_k16</t>
@@ -57,10 +57,10 @@
     <t>layer_label</t>
   </si>
   <si>
-    <t>k9_confidence</t>
-  </si>
-  <si>
-    <t>k9_label</t>
+    <t>k09_confidence</t>
+  </si>
+  <si>
+    <t>k09_label</t>
   </si>
   <si>
     <t>k16_confidence</t>
@@ -222,127 +222,121 @@
     <t>WM</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5/3</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>4/8/5/7</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>8/5</t>
-  </si>
-  <si>
-    <t>8/5/4</t>
-  </si>
-  <si>
-    <t>8/4/5</t>
-  </si>
-  <si>
-    <t>5/3/8</t>
-  </si>
-  <si>
-    <t>2*</t>
-  </si>
-  <si>
-    <t>3/5</t>
-  </si>
-  <si>
-    <t>3*</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1/6/2</t>
-  </si>
-  <si>
-    <t>6/9</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>6/2</t>
-  </si>
-  <si>
-    <t>14/2</t>
-  </si>
-  <si>
-    <t>8/3/9</t>
-  </si>
-  <si>
-    <t>7/4/9</t>
-  </si>
-  <si>
-    <t>9/4/7/16/5/3</t>
-  </si>
-  <si>
-    <t>4/16/7/9/5/12</t>
-  </si>
-  <si>
-    <t>3/9/5/8/10/7/16/4</t>
-  </si>
-  <si>
-    <t>4/16/7/12</t>
-  </si>
-  <si>
-    <t>5/3/9/16/4/7</t>
-  </si>
-  <si>
-    <t>5/9/3/16/4/7</t>
-  </si>
-  <si>
-    <t>9/4/3/5/16/7/8/10/12</t>
-  </si>
-  <si>
-    <t>9/4/5/3/7/16/8/10/12</t>
-  </si>
-  <si>
-    <t>5/16/3/9/4/12/7</t>
-  </si>
-  <si>
-    <t>9/3/5/8/7/16/4/10</t>
-  </si>
-  <si>
-    <t>8/10/3</t>
-  </si>
-  <si>
-    <t>5/9/16/4/3</t>
-  </si>
-  <si>
-    <t>10/3/8/5/16/9</t>
-  </si>
-  <si>
-    <t>8*</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>6/15/1/14/11</t>
-  </si>
-  <si>
-    <t>15/6/11/13</t>
-  </si>
-  <si>
-    <t>6/15</t>
-  </si>
-  <si>
-    <t>6/15/11/13</t>
+    <t>Sp09D02</t>
+  </si>
+  <si>
+    <t>Sp09D01</t>
+  </si>
+  <si>
+    <t>Sp09D05/Sp09D03</t>
+  </si>
+  <si>
+    <t>Sp09D07</t>
+  </si>
+  <si>
+    <t>Sp09D04/Sp09D08/Sp09D05/Sp09D07</t>
+  </si>
+  <si>
+    <t>Sp09D04</t>
+  </si>
+  <si>
+    <t>Sp09D05</t>
+  </si>
+  <si>
+    <t>Sp09D08/Sp09D05</t>
+  </si>
+  <si>
+    <t>Sp09D08/Sp09D04</t>
+  </si>
+  <si>
+    <t>Sp09D08</t>
+  </si>
+  <si>
+    <t>Sp09D02*</t>
+  </si>
+  <si>
+    <t>Sp09D03</t>
+  </si>
+  <si>
+    <t>Sp09D05/Sp09D03/Sp09D08</t>
+  </si>
+  <si>
+    <t>Sp09D03*</t>
+  </si>
+  <si>
+    <t>Sp09D01/Sp09D06</t>
+  </si>
+  <si>
+    <t>Sp09D06/Sp09D09</t>
+  </si>
+  <si>
+    <t>Sp09D06</t>
+  </si>
+  <si>
+    <t>Sp16D14/Sp16D02</t>
+  </si>
+  <si>
+    <t>Sp16D01</t>
+  </si>
+  <si>
+    <t>Sp16D08/Sp16D03/Sp16D09</t>
+  </si>
+  <si>
+    <t>Sp16D07</t>
+  </si>
+  <si>
+    <t>Sp16D09/Sp16D04</t>
+  </si>
+  <si>
+    <t>Sp16D04</t>
+  </si>
+  <si>
+    <t>Sp16D03</t>
+  </si>
+  <si>
+    <t>Sp16D05/Sp16D03/Sp16D09/Sp16D16</t>
+  </si>
+  <si>
+    <t>Sp16D05/Sp16D09/Sp16D03/Sp16D16/Sp16D04</t>
+  </si>
+  <si>
+    <t>Sp16D09</t>
+  </si>
+  <si>
+    <t>Sp16D09/Sp16D04/Sp16D05</t>
+  </si>
+  <si>
+    <t>Sp16D05</t>
+  </si>
+  <si>
+    <t>Sp16D09/Sp16D03</t>
+  </si>
+  <si>
+    <t>Sp16D02*</t>
+  </si>
+  <si>
+    <t>Sp16D08/Sp16D10/Sp16D03</t>
+  </si>
+  <si>
+    <t>Sp16D05/Sp16D09/Sp16D16</t>
+  </si>
+  <si>
+    <t>Sp16D10/Sp16D03/Sp16D08/Sp16D05/Sp16D16/Sp16D09</t>
+  </si>
+  <si>
+    <t>Sp16D08*</t>
+  </si>
+  <si>
+    <t>Sp16D08</t>
+  </si>
+  <si>
+    <t>Sp16D06</t>
+  </si>
+  <si>
+    <t>Sp16D15/Sp16D06/Sp16D11</t>
+  </si>
+  <si>
+    <t>Sp16D06/Sp16D15</t>
   </si>
   <si>
     <t>L3/4/5</t>
@@ -354,6 +348,9 @@
     <t>L3/4</t>
   </si>
   <si>
+    <t>L1/WM</t>
+  </si>
+  <si>
     <t>EndoMural</t>
   </si>
   <si>
@@ -402,28 +399,31 @@
     <t>Layer1</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
+    <t>Sp09D09</t>
+  </si>
+  <si>
+    <t>Sp16D02</t>
+  </si>
+  <si>
+    <t>Sp16D10</t>
+  </si>
+  <si>
+    <t>Sp16D11</t>
+  </si>
+  <si>
+    <t>Sp16D12</t>
+  </si>
+  <si>
+    <t>Sp16D13</t>
+  </si>
+  <si>
+    <t>Sp16D14</t>
+  </si>
+  <si>
+    <t>Sp16D15</t>
+  </si>
+  <si>
+    <t>Sp16D16</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
         <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>50</v>
@@ -605,13 +605,13 @@
         <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
         <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
@@ -634,13 +634,13 @@
         <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
         <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5">
@@ -663,13 +663,13 @@
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
@@ -692,13 +692,13 @@
         <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
         <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7">
@@ -721,13 +721,13 @@
         <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
         <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
@@ -750,13 +750,13 @@
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
         <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
@@ -779,13 +779,13 @@
         <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
@@ -808,13 +808,13 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11">
@@ -837,13 +837,13 @@
         <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
         <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12">
@@ -866,13 +866,13 @@
         <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s">
         <v>55</v>
       </c>
       <c r="I12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
@@ -895,13 +895,13 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14">
@@ -924,13 +924,13 @@
         <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H14" t="s">
         <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15">
@@ -947,19 +947,19 @@
         <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
         <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16">
@@ -976,13 +976,13 @@
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
         <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H16" t="s">
         <v>58</v>
@@ -1005,16 +1005,16 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
         <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I17" t="e">
         <v>#N/A</v>
@@ -1034,19 +1034,19 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
         <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H18" t="s">
         <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19">
@@ -1063,13 +1063,13 @@
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
         <v>61</v>
@@ -1092,19 +1092,19 @@
         <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
         <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" t="s">
         <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21">
@@ -1127,13 +1127,13 @@
         <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" t="s">
         <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22">
@@ -1150,19 +1150,19 @@
         <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
         <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23">
@@ -1185,13 +1185,13 @@
         <v>49</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" t="s">
         <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
@@ -1208,19 +1208,19 @@
         <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
         <v>48</v>
       </c>
       <c r="G24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" t="s">
         <v>65</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25">
@@ -1243,13 +1243,13 @@
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" t="s">
         <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
@@ -1266,16 +1266,16 @@
         <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
         <v>48</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="I26" t="s">
         <v>43</v>
@@ -1295,19 +1295,19 @@
         <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
         <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H27" t="s">
         <v>67</v>
       </c>
       <c r="I27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1324,19 +1324,19 @@
         <v>48</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
         <v>48</v>
       </c>
       <c r="G28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H28" t="s">
         <v>67</v>
       </c>
       <c r="I28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -1353,19 +1353,19 @@
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
         <v>48</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H29" t="s">
         <v>67</v>
       </c>
       <c r="I29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -1382,16 +1382,16 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
         <v>48</v>
       </c>
       <c r="G30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="I30" t="s">
         <v>47</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" t="n">
         <v>0.031103212903367445</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="n">
         <v>-0.18337511094156497</v>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" t="n">
         <v>-0.15863033472459015</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" t="n">
         <v>-0.31242125360162476</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" t="n">
         <v>-0.29996945156214855</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8" t="n">
         <v>-0.009711554190623941</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
         <v>-0.41457774970461775</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="n">
         <v>0.5241673247685127</v>
@@ -2893,7 +2893,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B9" t="n">
         <v>-0.16854009084281374</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" t="n">
         <v>0.4794176842787932</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B2" t="n">
         <v>0.7347806795869234</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="B3" t="n">
         <v>0.28782064313541156</v>
@@ -3364,7 +3364,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B4" t="n">
         <v>-0.36404083969584033</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B5" t="n">
         <v>-0.4803037253077219</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B6" t="n">
         <v>-0.4068068678812917</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="B7" t="n">
         <v>0.2929891028645663</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B8" t="n">
         <v>-0.4983073120319316</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="n">
         <v>-0.2820722134334666</v>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B10" t="n">
         <v>-0.49211855507062024</v>

</xml_diff>